<commit_message>
My first after adding My part at night after playing holi
</commit_message>
<xml_diff>
--- a/backend/slack-hrbp/Attendance_Report_2025-02.xlsx
+++ b/backend/slack-hrbp/Attendance_Report_2025-02.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>User Name</t>
   </si>
@@ -53,16 +53,25 @@
     <t>Feb-28</t>
   </si>
   <si>
+    <t>Varun</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
     <t>R Rohit</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Jagadeesh Latti</t>
   </si>
   <si>
-    <t>P</t>
+    <t>U</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
   <si>
     <t>S</t>
@@ -113,7 +122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -195,18 +204,18 @@
         <v>14</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>14</v>
@@ -215,31 +224,72 @@
         <v>14</v>
       </c>
       <c r="E3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="B4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s" s="0">
+      <c r="D4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="L3" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="M3" t="s" s="0">
-        <v>16</v>
+      <c r="H4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>